<commit_message>
add command to reach main branch to the develop branch in Git command file
</commit_message>
<xml_diff>
--- a/GIT_Command/Git_Usful_Commands.xlsx
+++ b/GIT_Command/Git_Usful_Commands.xlsx
@@ -5,38 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programing_Practice\GIT_Command\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\GIT_Command\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5DD7641-DF94-4185-BA16-C81CF0707782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3666C3-2662-4251-A524-83A9BC5B99D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5334ED2-4619-4007-B3F0-CA5844466EA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ردیف</t>
   </si>
@@ -50,22 +39,44 @@
     <t>با این دستور شما همه ی شاخه ها را می بینید</t>
   </si>
   <si>
-    <t>با این دستور شاخه ی develop به شاخه main وارد شد و تغییرات در اکانت github مشاهده شد</t>
-  </si>
-  <si>
     <t>git branch -a</t>
   </si>
   <si>
     <t>git push origin develop:main</t>
+  </si>
+  <si>
+    <t>git push origin develop</t>
+  </si>
+  <si>
+    <t>git switch main</t>
+  </si>
+  <si>
+    <t>git merge develop</t>
+  </si>
+  <si>
+    <t>git push origin main</t>
+  </si>
+  <si>
+    <t>در این دستورات اگه شاخه اصلی ما (main) از شاخه توسعه ما (develop) عقب باشد ، به آن می رسد . اول از همه بعد از commit کردن در شاخه develop آن را به داخل خود شاخه develop وارد (push) می کنیم و سپس به شاخه اصلی جا به جا می شویم با دستور switch سپس main را با develop ادغام (merge) می کنیم و اگر در این مرحله خطایی (conflict) مشاهده نشد دستور نهایی که وارد کردن تغییرات آخرین نسخه ی شاخه توسعه به داخل شاخه اصلی را انجام می دهیم و دیگر شاخه ی اصلی ما به توسعه ما یکی است</t>
+  </si>
+  <si>
+    <t xml:space="preserve">با این دستور شاخه ی develop به شاخه main وارد شد و تغییرات در اکانت github مشاهده شد . ولی در گیت گراف همچنان شاخه اصلی از شاخه ی توسعه عقب بود . چرا ؟ نمیدانم ! اگر میخواهید در گیت گراف هم درست باشد باید دستورات زیر را انجام دهید . </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -92,8 +103,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,24 +428,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB8ED21-3D38-4061-AB2E-4CA09D2A9D94}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -433,29 +453,98 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:C7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>